<commit_message>
feat: Convert Job Engine and Job Profile tabs to light theme
- Job Engine: Browser simulation, status bar, job cards
- Job Profile: Header, progress bar, personal info, Naukri credentials
- Update all dark theme colors to light theme equivalents
- Use primary-500/purple-500 for accents instead of neon colors
- White backgrounds with gray borders and shadows
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-09T21:45:57.123Z</v>
+        <v>2026-01-10T14:12:56.738Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-micro-wings-mumbai-all-areas-2-to-7-years-180925000269</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-divergentsoft-lab-indore-3-to-8-years-090126024501</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
@@ -526,48 +526,51 @@
         <v>Java Full Stack Developer</v>
       </c>
       <c r="N2" t="str">
-        <v>Micro Wings</v>
+        <v>DivergentSoft lab</v>
       </c>
       <c r="O2" t="str">
-        <v>2 - 7 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P2" t="str">
-        <v>3-6 Lacs P.A.</v>
+        <v>0 P.A.</v>
       </c>
       <c r="Q2" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Indore( Vijay Nagar )</v>
       </c>
       <c r="R2" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S2" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T2" t="str">
-        <v>100+</v>
+        <v>37</v>
       </c>
       <c r="U2" t="str">
-        <v>Java, Hibernate, Spring Boot, Java Fullstack, Angular, Debugging Skills, Cross Functional Coordination, Maven, Spring Mvc, SOAP UI, Postgresql, HTML, Oops Programming, JIRA, Microservices, JUnit, JSP Servlets, Postman Tool, Java Development, Restful Web Api Development</v>
+        <v>Full Stack, Spring Boot, Java Fullstack, Angular, React.Js, Node.Js, HTML, SQL, Reacts Js, English, Typescript, MySQL, Javascript, MongoDB</v>
       </c>
       <c r="V2" t="str">
-        <v>Full Stack Developer</v>
+        <v>Technology / IT - Other</v>
       </c>
       <c r="W2" t="str">
-        <v>Software Product</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="X2" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y2" t="str">
-        <v>Software Development</v>
+        <v>Technology / IT</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>3.5</v>
       </c>
       <c r="AA2" t="str">
-        <v>Proficient in Java, Spring Boot, Hibernate, Angular, and SQL | Develop and integrate SOAP/REST services, manage transactions, and perform debugging</v>
+        <v>Experience with Java 8/17, Spring Boot, Microservices, and frontend technologies like Angular/React | Develop REST APIs and work in an Agile environment using Git | Provident fund included</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2026-01-09T21:46:00.411Z</v>
+        <v>2026-01-10T14:13:00.029Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -576,7 +579,7 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-opus-pune-2-to-5-years-080126504723</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-micro-wings-mumbai-all-areas-2-to-7-years-180925000269</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
@@ -585,19 +588,19 @@
         <v>Yes</v>
       </c>
       <c r="G3" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H3" t="str">
         <v>Yes</v>
       </c>
       <c r="I3" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J3" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K3" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L3" t="str">
         <v>Skipped</v>
@@ -606,34 +609,34 @@
         <v>Java Full Stack Developer</v>
       </c>
       <c r="N3" t="str">
-        <v>Opus Technosoft</v>
+        <v>Micro Wings</v>
       </c>
       <c r="O3" t="str">
-        <v>2 - 5 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="P3" t="str">
-        <v>Not Disclosed</v>
+        <v>3-6 Lacs P.A.</v>
       </c>
       <c r="Q3" t="str">
-        <v>Pune</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R3" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S3" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T3" t="str">
         <v>100+</v>
       </c>
       <c r="U3" t="str">
-        <v>SAN, Front end, French, GIT, Shaping, MySQL, Javascript, HTML, payment solutions, Monitoring</v>
+        <v>Java, Hibernate, Spring Boot, Java Fullstack, Angular, Debugging Skills, Cross Functional Coordination, Maven, Spring Mvc, SOAP UI, Postgresql, HTML, Oops Programming, JIRA, Microservices, JUnit, JSP Servlets, Postman Tool, Java Development, Restful Web Api Development</v>
       </c>
       <c r="V3" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W3" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Software Product</v>
       </c>
       <c r="X3" t="str">
         <v>Full Time, Permanent</v>
@@ -642,12 +645,12 @@
         <v>Software Development</v>
       </c>
       <c r="AA3" t="str">
-        <v>Required Skills &amp; Experience . Strong proficiency in Java and Angular | Experience with version control systems (Git and BitBucket) | Experience with Postman for API testing and JUnit for unit testing . Hands-on experience with Keycloak (authentication &amp; authorization) and Kibana (log monitoring &amp; analytics) | Experience with AWS cloud services</v>
+        <v>Proficient in Java, Spring Boot, Hibernate, Angular, and SQL | Develop and integrate SOAP/REST services, manage transactions, and perform debugging</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2026-01-09T21:46:03.678Z</v>
+        <v>2026-01-10T14:13:03.359Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -701,7 +704,7 @@
         <v>1 day ago</v>
       </c>
       <c r="S4" t="str">
-        <v>Less than 10</v>
+        <v>14</v>
       </c>
       <c r="U4" t="str">
         <v>software engineer, github, restful, api gateway, html5, full stack developer, redis, nosql, sql, microservices, docker, angular, spring boot, java, restful apis, git, postgresql, full stack, mysql, typescript, agile, mongodb, css3, architecture</v>
@@ -727,7 +730,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2026-01-09T21:46:06.979Z</v>
+        <v>2026-01-10T14:13:06.654Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -736,16 +739,16 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-grid-dynamics-bengaluru-3-to-5-years-080126501444</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-capital-business-systems-prayagraj-3-to-7-years-090126011977</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
       </c>
       <c r="F5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G5" t="str">
         <v>No</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Yes</v>
       </c>
       <c r="H5" t="str">
         <v>Yes</v>
@@ -757,7 +760,7 @@
         <v>Poor Match</v>
       </c>
       <c r="K5" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L5" t="str">
         <v>Skipped</v>
@@ -766,16 +769,16 @@
         <v>Java Full Stack Developer</v>
       </c>
       <c r="N5" t="str">
-        <v>Grid Dynamics</v>
+        <v>Capital Business Systems</v>
       </c>
       <c r="O5" t="str">
-        <v>3 - 5 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P5" t="str">
-        <v>Not Disclosed</v>
+        <v>5-10 Lacs P.A.</v>
       </c>
       <c r="Q5" t="str">
-        <v>Bengaluru</v>
+        <v>Prayagraj</v>
       </c>
       <c r="R5" t="str">
         <v>1 day ago</v>
@@ -784,10 +787,10 @@
         <v>1</v>
       </c>
       <c r="T5" t="str">
-        <v>50+</v>
+        <v>100+</v>
       </c>
       <c r="U5" t="str">
-        <v>Backend, Db2, XML, MySQL, Data structures, Data processing, JSON, Oracle, Financial services</v>
+        <v>Java, Angular, Hibernate, Postgresql, MySQL, Spring Boot, J2Ee, Java Fullstack, Spring, Microservices</v>
       </c>
       <c r="V5" t="str">
         <v>Full Stack Developer</v>
@@ -802,15 +805,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z5" t="str">
-        <v>3.0</v>
+        <v>3.6</v>
       </c>
       <c r="AA5" t="str">
-        <v/>
+        <v>Full-stack developer with hands-on experience in Java (J2EE, Spring Boot, Hibernate) and modern front-end frameworks like Angular or React | Develop front-end interfaces, build back-end services, design RESTful APIs, manage databases, and deploy applications using DevOps tools</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2026-01-09T21:46:10.282Z</v>
+        <v>2026-01-10T14:13:10.051Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -819,7 +822,7 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-capital-business-systems-prayagraj-3-to-7-years-090126011977</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126931488</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
@@ -828,49 +831,46 @@
         <v>Yes</v>
       </c>
       <c r="G6" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H6" t="str">
         <v>Yes</v>
       </c>
       <c r="I6" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J6" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K6" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L6" t="str">
         <v>Skipped</v>
       </c>
       <c r="M6" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="N6" t="str">
-        <v>Capital Business Systems</v>
+        <v>Accenture</v>
       </c>
       <c r="O6" t="str">
-        <v>3 - 7 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P6" t="str">
-        <v>5-10 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q6" t="str">
-        <v>Prayagraj</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R6" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S6" t="str">
-        <v>1</v>
-      </c>
-      <c r="T6" t="str">
-        <v>100+</v>
+        <v>12</v>
       </c>
       <c r="U6" t="str">
-        <v>Java, Angular, Hibernate, Postgresql, MySQL, Spring Boot, J2Ee, Java Fullstack, Spring, Microservices</v>
+        <v>software engineer, front end, css, api development, restful, full stack development, version control, front end technologies, javascript, spring boot, java, git, design, full stack, software solutions, html, agile</v>
       </c>
       <c r="V6" t="str">
         <v>Full Stack Developer</v>
@@ -885,15 +885,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z6" t="str">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="AA6" t="str">
-        <v>Full-stack developer with hands-on experience in Java (J2EE, Spring Boot, Hibernate) and modern front-end frameworks like Angular or React | Develop front-end interfaces, build back-end services, design RESTful APIs, manage databases, and deploy applications using DevOps tools</v>
+        <v>Minimum 2 years experience in Java Full Stack Development; proficiency in front-end technologies and RESTful API integration | Develop custom software solutions, collaborate with teams, and assist in documentation</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2026-01-09T21:46:13.574Z</v>
+        <v>2026-01-10T14:13:13.419Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -902,7 +902,7 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-3i-infotech-mumbai-all-areas-2-to-7-years-080126016500</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930110</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
@@ -911,52 +911,49 @@
         <v>Yes</v>
       </c>
       <c r="G7" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H7" t="str">
         <v>Yes</v>
       </c>
       <c r="I7" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J7" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K7" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L7" t="str">
         <v>Skipped</v>
       </c>
       <c r="M7" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="N7" t="str">
-        <v>3i Infotech</v>
+        <v>Accenture</v>
       </c>
       <c r="O7" t="str">
-        <v>2 - 7 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P7" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q7" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R7" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S7" t="str">
-        <v>1</v>
-      </c>
-      <c r="T7" t="str">
-        <v>100+</v>
+        <v>Less than 10</v>
       </c>
       <c r="U7" t="str">
-        <v>React.Js, Angular, Java Spring Boot, HTML, Java Fullstack, AWS</v>
+        <v>software engineer, front end, kubernetes, css, api development, javascript, nosql, sql, docker, angular, spring boot, back end, database management, java, git, oops, full stack, web development, typescript, agile, aws, nosql databases</v>
       </c>
       <c r="V7" t="str">
-        <v>Software Development - Other</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W7" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -968,15 +965,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z7" t="str">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="AA7" t="str">
-        <v>Bachelor's degree in Computer Science or related field with 3+ years of experience in Java Full Stack Development | Design, develop, and maintain full-stack web applications using Java and modern frameworks; develop backend services and build responsive frontend interfaces</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern frameworks like Spring and Angular | Design, develop, and maintain web applications; collaborate with teams to deliver scalable solutions</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2026-01-09T21:46:16.919Z</v>
+        <v>2026-01-10T14:13:16.710Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -985,7 +982,7 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-3i-infotech-hyderabad-mumbai-all-areas-3-to-8-years-080126010394</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930493</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
@@ -1006,37 +1003,34 @@
         <v>Good Match</v>
       </c>
       <c r="K8" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L8" t="str">
-        <v>Applied</v>
+        <v>Skipped</v>
       </c>
       <c r="M8" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Custom Software Engineer</v>
       </c>
       <c r="N8" t="str">
-        <v>3i Infotech</v>
+        <v>Accenture</v>
       </c>
       <c r="O8" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P8" t="str">
-        <v>13-23 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q8" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R8" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S8" t="str">
-        <v>8</v>
-      </c>
-      <c r="T8" t="str">
-        <v>100+</v>
+        <v>Less than 10</v>
       </c>
       <c r="U8" t="str">
-        <v>Java, Spring Boot, API, React.Js, Angular, SQL</v>
+        <v>software engineer, restful, nosql, sql, microservices, web development frameworks, angular, database management, java, restful apis, git, microservices architecture, full stack, web development, agile, architecture, nosql databases</v>
       </c>
       <c r="V8" t="str">
         <v>Full Stack Developer</v>
@@ -1051,15 +1045,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z8" t="str">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="AA8" t="str">
-        <v>Bachelor’s degree in Computer Science or Engineering; strong proficiency in Java, Spring Boot, and modern frontend frameworks like Angular or React | Design, develop, and maintain full stack web applications; develop backend services and RESTful APIs; build responsive UI components</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, and enhance development processes</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2026-01-09T21:46:46.923Z</v>
+        <v>2026-01-10T14:13:19.984Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1068,7 +1062,7 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126931488</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-090126931461</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
@@ -1107,7 +1101,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q9" t="str">
-        <v>Hyderabad</v>
+        <v>Pune</v>
       </c>
       <c r="R9" t="str">
         <v>1 day ago</v>
@@ -1116,7 +1110,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U9" t="str">
-        <v>software engineer, front end, css, api development, restful, full stack development, version control, front end technologies, javascript, spring boot, java, git, design, full stack, software solutions, html, agile</v>
+        <v>software engineer, restful, software development, full stack development, version control, nosql, sql, angular, database management, java, git, web frameworks, api design, design, full stack, software solutions, agile, nosql databases</v>
       </c>
       <c r="V9" t="str">
         <v>Full Stack Developer</v>
@@ -1134,12 +1128,12 @@
         <v>3.7</v>
       </c>
       <c r="AA9" t="str">
-        <v>Minimum 2 years experience in Java Full Stack Development; proficiency in front-end technologies and RESTful API integration | Develop custom software solutions, collaborate with teams, and assist in documentation</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern web frameworks like Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2026-01-09T21:46:50.246Z</v>
+        <v>2026-01-10T14:13:23.388Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1148,7 +1142,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930110</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-090126930317</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1187,7 +1181,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q10" t="str">
-        <v>Bengaluru</v>
+        <v>Chennai</v>
       </c>
       <c r="R10" t="str">
         <v>1 day ago</v>
@@ -1196,7 +1190,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U10" t="str">
-        <v>software engineer, front end, kubernetes, css, api development, javascript, nosql, sql, docker, angular, spring boot, back end, database management, java, git, oops, full stack, web development, typescript, agile, aws, nosql databases</v>
+        <v>software engineer, restful, software development, nosql, sql, web development frameworks, angular, database management, java, git, api design, full stack, agile methodologies, software solutions, web development, agile, nosql databases</v>
       </c>
       <c r="V10" t="str">
         <v>Full Stack Developer</v>
@@ -1214,12 +1208,12 @@
         <v>3.7</v>
       </c>
       <c r="AA10" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern frameworks like Spring and Angular | Design, develop, and maintain web applications; collaborate with teams to deliver scalable solutions</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2026-01-09T21:46:53.561Z</v>
+        <v>2026-01-10T14:13:26.719Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1228,7 +1222,7 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-090126931461</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930328</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
@@ -1261,13 +1255,13 @@
         <v>Accenture</v>
       </c>
       <c r="O11" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P11" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q11" t="str">
-        <v>Pune</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R11" t="str">
         <v>1 day ago</v>
@@ -1276,7 +1270,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U11" t="str">
-        <v>software engineer, restful, software development, full stack development, version control, nosql, sql, angular, database management, java, git, web frameworks, api design, design, full stack, software solutions, agile, nosql databases</v>
+        <v>software engineer, restful, react, sql, microservices, java, git, webpack, kanban, mysql, mongodb, programming, azure, front end, oracle, software development, npm, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
       </c>
       <c r="V11" t="str">
         <v>Full Stack Developer</v>
@@ -1294,12 +1288,12 @@
         <v>3.7</v>
       </c>
       <c r="AA11" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern web frameworks like Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with strong proficiency in Java and React.js | Design, develop, and maintain Java-based applications and microservices; collaborate in agile software development</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2026-01-09T21:46:57.181Z</v>
+        <v>2026-01-10T14:13:30.004Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1308,7 +1302,7 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-090126930317</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-090126930803</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
@@ -1341,7 +1335,7 @@
         <v>Accenture</v>
       </c>
       <c r="O12" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P12" t="str">
         <v>Not Disclosed</v>
@@ -1356,7 +1350,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U12" t="str">
-        <v>software engineer, restful, software development, nosql, sql, web development frameworks, angular, database management, java, git, api design, full stack, agile methodologies, software solutions, web development, agile, nosql databases</v>
+        <v>software engineer, front end, application developer, css, restful, business processes, agile development, hibernate, javascript, sql, spring framework, database management, java, full stack, software solutions, construction, html, agile</v>
       </c>
       <c r="V12" t="str">
         <v>Full Stack Developer</v>
@@ -1374,12 +1368,12 @@
         <v>3.7</v>
       </c>
       <c r="AA12" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in front-end technologies | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2026-01-09T21:47:00.548Z</v>
+        <v>2026-01-10T14:13:33.292Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1388,7 +1382,7 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930328</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-2-to-5-years-090126931479</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
@@ -1421,13 +1415,13 @@
         <v>Accenture</v>
       </c>
       <c r="O13" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P13" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q13" t="str">
-        <v>Bengaluru</v>
+        <v>Gurugram</v>
       </c>
       <c r="R13" t="str">
         <v>1 day ago</v>
@@ -1436,7 +1430,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U13" t="str">
-        <v>software engineer, restful, react, sql, microservices, java, git, webpack, kanban, mysql, mongodb, programming, azure, front end, oracle, software development, npm, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
+        <v>software engineer, front end, css, full stack development, version control, front end technologies, hibernate, javascript, nosql, sql, back end, database management, java, git, design, full stack, software solutions, html, agile, nosql databases</v>
       </c>
       <c r="V13" t="str">
         <v>Full Stack Developer</v>
@@ -1454,12 +1448,12 @@
         <v>3.7</v>
       </c>
       <c r="AA13" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with strong proficiency in Java and React.js | Design, develop, and maintain Java-based applications and microservices; collaborate in agile software development</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in front-end technologies and back-end frameworks | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2026-01-09T21:47:03.818Z</v>
+        <v>2026-01-10T14:13:36.642Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1468,7 +1462,7 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-090126930803</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-indore-3-to-8-years-090126931329</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
@@ -1477,16 +1471,16 @@
         <v>Yes</v>
       </c>
       <c r="G14" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H14" t="str">
         <v>Yes</v>
       </c>
       <c r="I14" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J14" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K14" t="str">
         <v>External Apply</v>
@@ -1507,7 +1501,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q14" t="str">
-        <v>Chennai</v>
+        <v>Indore</v>
       </c>
       <c r="R14" t="str">
         <v>1 day ago</v>
@@ -1516,7 +1510,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U14" t="str">
-        <v>software engineer, front end, application developer, css, restful, business processes, agile development, hibernate, javascript, sql, spring framework, database management, java, full stack, software solutions, construction, html, agile</v>
+        <v>software engineer, front end, css, full stack development, version control, hibernate, javascript, web development frameworks, database management, java, git, postgresql, full stack, software solutions, mysql, web development, html, agile</v>
       </c>
       <c r="V14" t="str">
         <v>Full Stack Developer</v>
@@ -1534,12 +1528,12 @@
         <v>3.7</v>
       </c>
       <c r="AA14" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in front-end technologies | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in web development frameworks like Spring and Hibernate | Develop custom software solutions, collaborate with cross-functional teams, and engage in continuous learning</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2026-01-09T21:47:07.081Z</v>
+        <v>2026-01-10T14:13:40.080Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1548,7 +1542,7 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-indore-3-to-8-years-090126931329</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931192</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
@@ -1557,16 +1551,16 @@
         <v>Yes</v>
       </c>
       <c r="G15" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H15" t="str">
         <v>Yes</v>
       </c>
       <c r="I15" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J15" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K15" t="str">
         <v>External Apply</v>
@@ -1587,7 +1581,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q15" t="str">
-        <v>Indore</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R15" t="str">
         <v>1 day ago</v>
@@ -1596,7 +1590,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U15" t="str">
-        <v>software engineer, front end, css, full stack development, version control, hibernate, javascript, web development frameworks, database management, java, git, postgresql, full stack, software solutions, mysql, web development, html, agile</v>
+        <v>software engineer, rest, api development, restful, version control, user experience, sql, microservices, spring boot, database management, java, restful apis, git, microservices architecture, full stack, software solutions, agile, architecture</v>
       </c>
       <c r="V15" t="str">
         <v>Full Stack Developer</v>
@@ -1614,12 +1608,12 @@
         <v>3.7</v>
       </c>
       <c r="AA15" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in web development frameworks like Spring and Hibernate | Develop custom software solutions, collaborate with cross-functional teams, and engage in continuous learning</v>
+        <v>Minimum 3 years of experience in Spring Boot; BTech, MTech, or MCA in IT, CSE, EEE, or ECE | Develop custom software solutions and RESTful APIs; Collaborate with cross-functional teams and stakeholders</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2026-01-09T21:47:10.417Z</v>
+        <v>2026-01-10T14:13:43.386Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1628,7 +1622,7 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931192</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126930327</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
@@ -1661,7 +1655,7 @@
         <v>Accenture</v>
       </c>
       <c r="O16" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P16" t="str">
         <v>Not Disclosed</v>
@@ -1676,7 +1670,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U16" t="str">
-        <v>software engineer, rest, api development, restful, version control, user experience, sql, microservices, spring boot, database management, java, restful apis, git, microservices architecture, full stack, software solutions, agile, architecture</v>
+        <v>software engineer, front end, css, full stack development, front end technologies, user experience, hibernate, javascript, nosql, sql, back end, database management, java, design, full stack, html, aws, nosql databases</v>
       </c>
       <c r="V16" t="str">
         <v>Full Stack Developer</v>
@@ -1694,12 +1688,12 @@
         <v>3.7</v>
       </c>
       <c r="AA16" t="str">
-        <v>Minimum 3 years of experience in Spring Boot; BTech, MTech, or MCA in IT, CSE, EEE, or ECE | Develop custom software solutions and RESTful APIs; Collaborate with cross-functional teams and stakeholders</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in front-end technologies | Lead design, build, and configuration of applications; collaborate with teams and ensure timely delivery</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2026-01-09T21:47:13.653Z</v>
+        <v>2026-01-10T14:13:46.621Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1708,7 +1702,7 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126930327</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931441</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
@@ -1741,7 +1735,7 @@
         <v>Accenture</v>
       </c>
       <c r="O17" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P17" t="str">
         <v>Not Disclosed</v>
@@ -1756,7 +1750,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U17" t="str">
-        <v>software engineer, front end, css, full stack development, front end technologies, user experience, hibernate, javascript, nosql, sql, back end, database management, java, design, full stack, html, aws, nosql databases</v>
+        <v>software engineer, front end, css, full stack development, version control, front end technologies, javascript, code quality, nosql, sql, spring boot, database management, java, git, full stack, software solutions, html, agile, nosql databases</v>
       </c>
       <c r="V17" t="str">
         <v>Full Stack Developer</v>
@@ -1774,12 +1768,12 @@
         <v>3.7</v>
       </c>
       <c r="AA17" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in front-end technologies | Lead design, build, and configuration of applications; collaborate with teams and ensure timely delivery</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development; proficiency in front-end technologies and database management | Develop custom software solutions, collaborate with teams, conduct code reviews</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2026-01-09T21:47:16.925Z</v>
+        <v>2026-01-10T14:13:49.940Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1788,7 +1782,7 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931441</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-090126931749</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
@@ -1827,7 +1821,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q18" t="str">
-        <v>Hyderabad</v>
+        <v>Gurugram</v>
       </c>
       <c r="R18" t="str">
         <v>1 day ago</v>
@@ -1836,7 +1830,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U18" t="str">
-        <v>software engineer, front end, css, full stack development, version control, front end technologies, javascript, code quality, nosql, sql, spring boot, database management, java, git, full stack, software solutions, html, agile, nosql databases</v>
+        <v>software engineer, front end, application developer, restful, web services, version control, business processes, react, angular, database management, java, git, postgresql, full stack, software solutions, debugging, construction, mysql, agile</v>
       </c>
       <c r="V18" t="str">
         <v>Full Stack Developer</v>
@@ -1854,12 +1848,12 @@
         <v>3.7</v>
       </c>
       <c r="AA18" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development; proficiency in front-end technologies and database management | Develop custom software solutions, collaborate with teams, conduct code reviews</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in RESTful web services and API integration | Develop custom software solutions, collaborate with teams, and ensure application performance</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2026-01-09T21:47:20.178Z</v>
+        <v>2026-01-10T14:13:53.257Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1868,7 +1862,7 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-090126931749</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930810</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
@@ -1907,7 +1901,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q19" t="str">
-        <v>Gurugram</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R19" t="str">
         <v>1 day ago</v>
@@ -1916,7 +1910,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U19" t="str">
-        <v>software engineer, front end, application developer, restful, web services, version control, business processes, react, angular, database management, java, git, postgresql, full stack, software solutions, debugging, construction, mysql, agile</v>
+        <v>software engineer, restful, full stack development, version control, database technologies, nosql, sql, web development frameworks, angular, java, git, api design, design, full stack, agile methodologies, software solutions, web development, agile</v>
       </c>
       <c r="V19" t="str">
         <v>Full Stack Developer</v>
@@ -1934,12 +1928,12 @@
         <v>3.7</v>
       </c>
       <c r="AA19" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in RESTful web services and API integration | Develop custom software solutions, collaborate with teams, and ensure application performance</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, and engage in code reviews</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2026-01-09T21:47:23.460Z</v>
+        <v>2026-01-10T14:13:56.598Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1993,7 +1987,7 @@
         <v>1 day ago</v>
       </c>
       <c r="S20" t="str">
-        <v>Less than 10</v>
+        <v>10</v>
       </c>
       <c r="U20" t="str">
         <v>software engineer, css, restful, react, sql, microservices, java, git, webpack, kanban, web development, azure, front end, oracle, software development, npm, javascript, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
@@ -2019,7 +2013,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2026-01-09T21:47:26.839Z</v>
+        <v>2026-01-10T14:13:59.959Z</v>
       </c>
       <c r="B21">
         <v>1</v>

</xml_diff>

<commit_message>
revert: Restore dark theme - user prefers original theme
- Revert Auth page to dark theme
- Revert Dashboard Sidebar to dark theme
- Revert Dashboard Layout to dark theme
- Revert Job Engine and Job Profile tabs to dark theme
- Keep icon.ico for Windows builds
- Keep all functionality improvements (animations, job cards UI)
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-10T14:12:56.738Z</v>
+        <v>2026-01-09T21:45:57.123Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-divergentsoft-lab-indore-3-to-8-years-090126024501</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-micro-wings-mumbai-all-areas-2-to-7-years-180925000269</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
@@ -526,51 +526,48 @@
         <v>Java Full Stack Developer</v>
       </c>
       <c r="N2" t="str">
-        <v>DivergentSoft lab</v>
+        <v>Micro Wings</v>
       </c>
       <c r="O2" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="P2" t="str">
-        <v>0 P.A.</v>
+        <v>3-6 Lacs P.A.</v>
       </c>
       <c r="Q2" t="str">
-        <v>Indore( Vijay Nagar )</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R2" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S2" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T2" t="str">
-        <v>37</v>
+        <v>100+</v>
       </c>
       <c r="U2" t="str">
-        <v>Full Stack, Spring Boot, Java Fullstack, Angular, React.Js, Node.Js, HTML, SQL, Reacts Js, English, Typescript, MySQL, Javascript, MongoDB</v>
+        <v>Java, Hibernate, Spring Boot, Java Fullstack, Angular, Debugging Skills, Cross Functional Coordination, Maven, Spring Mvc, SOAP UI, Postgresql, HTML, Oops Programming, JIRA, Microservices, JUnit, JSP Servlets, Postman Tool, Java Development, Restful Web Api Development</v>
       </c>
       <c r="V2" t="str">
-        <v>Technology / IT - Other</v>
+        <v>Full Stack Developer</v>
       </c>
       <c r="W2" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Software Product</v>
       </c>
       <c r="X2" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y2" t="str">
-        <v>Technology / IT</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>3.5</v>
+        <v>Software Development</v>
       </c>
       <c r="AA2" t="str">
-        <v>Experience with Java 8/17, Spring Boot, Microservices, and frontend technologies like Angular/React | Develop REST APIs and work in an Agile environment using Git | Provident fund included</v>
+        <v>Proficient in Java, Spring Boot, Hibernate, Angular, and SQL | Develop and integrate SOAP/REST services, manage transactions, and perform debugging</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2026-01-10T14:13:00.029Z</v>
+        <v>2026-01-09T21:46:00.411Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -579,7 +576,7 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-micro-wings-mumbai-all-areas-2-to-7-years-180925000269</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-opus-pune-2-to-5-years-080126504723</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
@@ -588,19 +585,19 @@
         <v>Yes</v>
       </c>
       <c r="G3" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H3" t="str">
         <v>Yes</v>
       </c>
       <c r="I3" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J3" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K3" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L3" t="str">
         <v>Skipped</v>
@@ -609,34 +606,34 @@
         <v>Java Full Stack Developer</v>
       </c>
       <c r="N3" t="str">
-        <v>Micro Wings</v>
+        <v>Opus Technosoft</v>
       </c>
       <c r="O3" t="str">
-        <v>2 - 7 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P3" t="str">
-        <v>3-6 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q3" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Pune</v>
       </c>
       <c r="R3" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S3" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T3" t="str">
         <v>100+</v>
       </c>
       <c r="U3" t="str">
-        <v>Java, Hibernate, Spring Boot, Java Fullstack, Angular, Debugging Skills, Cross Functional Coordination, Maven, Spring Mvc, SOAP UI, Postgresql, HTML, Oops Programming, JIRA, Microservices, JUnit, JSP Servlets, Postman Tool, Java Development, Restful Web Api Development</v>
+        <v>SAN, Front end, French, GIT, Shaping, MySQL, Javascript, HTML, payment solutions, Monitoring</v>
       </c>
       <c r="V3" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W3" t="str">
-        <v>Software Product</v>
+        <v>IT Services &amp; Consulting</v>
       </c>
       <c r="X3" t="str">
         <v>Full Time, Permanent</v>
@@ -645,12 +642,12 @@
         <v>Software Development</v>
       </c>
       <c r="AA3" t="str">
-        <v>Proficient in Java, Spring Boot, Hibernate, Angular, and SQL | Develop and integrate SOAP/REST services, manage transactions, and perform debugging</v>
+        <v>Required Skills &amp; Experience . Strong proficiency in Java and Angular | Experience with version control systems (Git and BitBucket) | Experience with Postman for API testing and JUnit for unit testing . Hands-on experience with Keycloak (authentication &amp; authorization) and Kibana (log monitoring &amp; analytics) | Experience with AWS cloud services</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2026-01-10T14:13:03.359Z</v>
+        <v>2026-01-09T21:46:03.678Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -704,7 +701,7 @@
         <v>1 day ago</v>
       </c>
       <c r="S4" t="str">
-        <v>14</v>
+        <v>Less than 10</v>
       </c>
       <c r="U4" t="str">
         <v>software engineer, github, restful, api gateway, html5, full stack developer, redis, nosql, sql, microservices, docker, angular, spring boot, java, restful apis, git, postgresql, full stack, mysql, typescript, agile, mongodb, css3, architecture</v>
@@ -730,7 +727,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2026-01-10T14:13:06.654Z</v>
+        <v>2026-01-09T21:46:06.979Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -739,16 +736,16 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-capital-business-systems-prayagraj-3-to-7-years-090126011977</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-grid-dynamics-bengaluru-3-to-5-years-080126501444</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
       </c>
       <c r="F5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G5" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H5" t="str">
         <v>Yes</v>
@@ -760,7 +757,7 @@
         <v>Poor Match</v>
       </c>
       <c r="K5" t="str">
-        <v>Direct Apply</v>
+        <v>External Apply</v>
       </c>
       <c r="L5" t="str">
         <v>Skipped</v>
@@ -769,16 +766,16 @@
         <v>Java Full Stack Developer</v>
       </c>
       <c r="N5" t="str">
-        <v>Capital Business Systems</v>
+        <v>Grid Dynamics</v>
       </c>
       <c r="O5" t="str">
-        <v>3 - 7 years</v>
+        <v>3 - 5 years</v>
       </c>
       <c r="P5" t="str">
-        <v>5-10 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q5" t="str">
-        <v>Prayagraj</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R5" t="str">
         <v>1 day ago</v>
@@ -787,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="T5" t="str">
-        <v>100+</v>
+        <v>50+</v>
       </c>
       <c r="U5" t="str">
-        <v>Java, Angular, Hibernate, Postgresql, MySQL, Spring Boot, J2Ee, Java Fullstack, Spring, Microservices</v>
+        <v>Backend, Db2, XML, MySQL, Data structures, Data processing, JSON, Oracle, Financial services</v>
       </c>
       <c r="V5" t="str">
         <v>Full Stack Developer</v>
@@ -805,15 +802,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z5" t="str">
-        <v>3.6</v>
+        <v>3.0</v>
       </c>
       <c r="AA5" t="str">
-        <v>Full-stack developer with hands-on experience in Java (J2EE, Spring Boot, Hibernate) and modern front-end frameworks like Angular or React | Develop front-end interfaces, build back-end services, design RESTful APIs, manage databases, and deploy applications using DevOps tools</v>
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2026-01-10T14:13:10.051Z</v>
+        <v>2026-01-09T21:46:10.282Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -822,7 +819,7 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126931488</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-capital-business-systems-prayagraj-3-to-7-years-090126011977</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
@@ -831,46 +828,49 @@
         <v>Yes</v>
       </c>
       <c r="G6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H6" t="str">
         <v>Yes</v>
       </c>
       <c r="I6" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J6" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K6" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L6" t="str">
         <v>Skipped</v>
       </c>
       <c r="M6" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Java Full Stack Developer</v>
       </c>
       <c r="N6" t="str">
-        <v>Accenture</v>
+        <v>Capital Business Systems</v>
       </c>
       <c r="O6" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P6" t="str">
-        <v>Not Disclosed</v>
+        <v>5-10 Lacs P.A.</v>
       </c>
       <c r="Q6" t="str">
-        <v>Hyderabad</v>
+        <v>Prayagraj</v>
       </c>
       <c r="R6" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S6" t="str">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="T6" t="str">
+        <v>100+</v>
       </c>
       <c r="U6" t="str">
-        <v>software engineer, front end, css, api development, restful, full stack development, version control, front end technologies, javascript, spring boot, java, git, design, full stack, software solutions, html, agile</v>
+        <v>Java, Angular, Hibernate, Postgresql, MySQL, Spring Boot, J2Ee, Java Fullstack, Spring, Microservices</v>
       </c>
       <c r="V6" t="str">
         <v>Full Stack Developer</v>
@@ -885,15 +885,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z6" t="str">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="AA6" t="str">
-        <v>Minimum 2 years experience in Java Full Stack Development; proficiency in front-end technologies and RESTful API integration | Develop custom software solutions, collaborate with teams, and assist in documentation</v>
+        <v>Full-stack developer with hands-on experience in Java (J2EE, Spring Boot, Hibernate) and modern front-end frameworks like Angular or React | Develop front-end interfaces, build back-end services, design RESTful APIs, manage databases, and deploy applications using DevOps tools</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2026-01-10T14:13:13.419Z</v>
+        <v>2026-01-09T21:46:13.574Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -902,7 +902,7 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930110</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-3i-infotech-mumbai-all-areas-2-to-7-years-080126016500</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
@@ -911,49 +911,52 @@
         <v>Yes</v>
       </c>
       <c r="G7" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H7" t="str">
         <v>Yes</v>
       </c>
       <c r="I7" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J7" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K7" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L7" t="str">
         <v>Skipped</v>
       </c>
       <c r="M7" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Java Full Stack Developer</v>
       </c>
       <c r="N7" t="str">
-        <v>Accenture</v>
+        <v>3i Infotech</v>
       </c>
       <c r="O7" t="str">
-        <v>2 - 5 years</v>
+        <v>2 - 7 years</v>
       </c>
       <c r="P7" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q7" t="str">
-        <v>Bengaluru</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R7" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S7" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T7" t="str">
+        <v>100+</v>
       </c>
       <c r="U7" t="str">
-        <v>software engineer, front end, kubernetes, css, api development, javascript, nosql, sql, docker, angular, spring boot, back end, database management, java, git, oops, full stack, web development, typescript, agile, aws, nosql databases</v>
+        <v>React.Js, Angular, Java Spring Boot, HTML, Java Fullstack, AWS</v>
       </c>
       <c r="V7" t="str">
-        <v>Full Stack Developer</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W7" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -965,15 +968,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z7" t="str">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="AA7" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern frameworks like Spring and Angular | Design, develop, and maintain web applications; collaborate with teams to deliver scalable solutions</v>
+        <v>Bachelor's degree in Computer Science or related field with 3+ years of experience in Java Full Stack Development | Design, develop, and maintain full-stack web applications using Java and modern frameworks; develop backend services and build responsive frontend interfaces</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2026-01-10T14:13:16.710Z</v>
+        <v>2026-01-09T21:46:16.919Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -982,7 +985,7 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930493</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developer-3i-infotech-hyderabad-mumbai-all-areas-3-to-8-years-080126010394</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
@@ -1003,34 +1006,37 @@
         <v>Good Match</v>
       </c>
       <c r="K8" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L8" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M8" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Java Full Stack Developer</v>
       </c>
       <c r="N8" t="str">
-        <v>Accenture</v>
+        <v>3i Infotech</v>
       </c>
       <c r="O8" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P8" t="str">
-        <v>Not Disclosed</v>
+        <v>13-23 Lacs P.A.</v>
       </c>
       <c r="Q8" t="str">
-        <v>Bengaluru</v>
+        <v>Mumbai (All Areas)</v>
       </c>
       <c r="R8" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S8" t="str">
-        <v>Less than 10</v>
+        <v>8</v>
+      </c>
+      <c r="T8" t="str">
+        <v>100+</v>
       </c>
       <c r="U8" t="str">
-        <v>software engineer, restful, nosql, sql, microservices, web development frameworks, angular, database management, java, restful apis, git, microservices architecture, full stack, web development, agile, architecture, nosql databases</v>
+        <v>Java, Spring Boot, API, React.Js, Angular, SQL</v>
       </c>
       <c r="V8" t="str">
         <v>Full Stack Developer</v>
@@ -1045,15 +1051,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z8" t="str">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="AA8" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, and enhance development processes</v>
+        <v>Bachelor’s degree in Computer Science or Engineering; strong proficiency in Java, Spring Boot, and modern frontend frameworks like Angular or React | Design, develop, and maintain full stack web applications; develop backend services and RESTful APIs; build responsive UI components</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2026-01-10T14:13:19.984Z</v>
+        <v>2026-01-09T21:46:46.923Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1062,7 +1068,7 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-090126931461</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126931488</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
@@ -1101,7 +1107,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q9" t="str">
-        <v>Pune</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R9" t="str">
         <v>1 day ago</v>
@@ -1110,7 +1116,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U9" t="str">
-        <v>software engineer, restful, software development, full stack development, version control, nosql, sql, angular, database management, java, git, web frameworks, api design, design, full stack, software solutions, agile, nosql databases</v>
+        <v>software engineer, front end, css, api development, restful, full stack development, version control, front end technologies, javascript, spring boot, java, git, design, full stack, software solutions, html, agile</v>
       </c>
       <c r="V9" t="str">
         <v>Full Stack Developer</v>
@@ -1128,12 +1134,12 @@
         <v>3.7</v>
       </c>
       <c r="AA9" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern web frameworks like Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>Minimum 2 years experience in Java Full Stack Development; proficiency in front-end technologies and RESTful API integration | Develop custom software solutions, collaborate with teams, and assist in documentation</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2026-01-10T14:13:23.388Z</v>
+        <v>2026-01-09T21:46:50.246Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1142,7 +1148,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-090126930317</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930110</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1181,7 +1187,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q10" t="str">
-        <v>Chennai</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R10" t="str">
         <v>1 day ago</v>
@@ -1190,7 +1196,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U10" t="str">
-        <v>software engineer, restful, software development, nosql, sql, web development frameworks, angular, database management, java, git, api design, full stack, agile methodologies, software solutions, web development, agile, nosql databases</v>
+        <v>software engineer, front end, kubernetes, css, api development, javascript, nosql, sql, docker, angular, spring boot, back end, database management, java, git, oops, full stack, web development, typescript, agile, aws, nosql databases</v>
       </c>
       <c r="V10" t="str">
         <v>Full Stack Developer</v>
@@ -1208,12 +1214,12 @@
         <v>3.7</v>
       </c>
       <c r="AA10" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern frameworks like Spring and Angular | Design, develop, and maintain web applications; collaborate with teams to deliver scalable solutions</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2026-01-10T14:13:26.719Z</v>
+        <v>2026-01-09T21:46:53.561Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1222,7 +1228,7 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930328</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-090126931461</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
@@ -1255,13 +1261,13 @@
         <v>Accenture</v>
       </c>
       <c r="O11" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P11" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q11" t="str">
-        <v>Bengaluru</v>
+        <v>Pune</v>
       </c>
       <c r="R11" t="str">
         <v>1 day ago</v>
@@ -1270,7 +1276,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U11" t="str">
-        <v>software engineer, restful, react, sql, microservices, java, git, webpack, kanban, mysql, mongodb, programming, azure, front end, oracle, software development, npm, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
+        <v>software engineer, restful, software development, full stack development, version control, nosql, sql, angular, database management, java, git, web frameworks, api design, design, full stack, software solutions, agile, nosql databases</v>
       </c>
       <c r="V11" t="str">
         <v>Full Stack Developer</v>
@@ -1288,12 +1294,12 @@
         <v>3.7</v>
       </c>
       <c r="AA11" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with strong proficiency in Java and React.js | Design, develop, and maintain Java-based applications and microservices; collaborate in agile software development</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern web frameworks like Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2026-01-10T14:13:30.004Z</v>
+        <v>2026-01-09T21:46:57.181Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1302,7 +1308,7 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-090126930803</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-090126930317</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
@@ -1335,7 +1341,7 @@
         <v>Accenture</v>
       </c>
       <c r="O12" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P12" t="str">
         <v>Not Disclosed</v>
@@ -1350,7 +1356,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U12" t="str">
-        <v>software engineer, front end, application developer, css, restful, business processes, agile development, hibernate, javascript, sql, spring framework, database management, java, full stack, software solutions, construction, html, agile</v>
+        <v>software engineer, restful, software development, nosql, sql, web development frameworks, angular, database management, java, git, api design, full stack, agile methodologies, software solutions, web development, agile, nosql databases</v>
       </c>
       <c r="V12" t="str">
         <v>Full Stack Developer</v>
@@ -1368,12 +1374,12 @@
         <v>3.7</v>
       </c>
       <c r="AA12" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in front-end technologies | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
+        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2026-01-10T14:13:33.292Z</v>
+        <v>2026-01-09T21:47:00.548Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1382,7 +1388,7 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-2-to-5-years-090126931479</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930328</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
@@ -1415,13 +1421,13 @@
         <v>Accenture</v>
       </c>
       <c r="O13" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P13" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q13" t="str">
-        <v>Gurugram</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R13" t="str">
         <v>1 day ago</v>
@@ -1430,7 +1436,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U13" t="str">
-        <v>software engineer, front end, css, full stack development, version control, front end technologies, hibernate, javascript, nosql, sql, back end, database management, java, git, design, full stack, software solutions, html, agile, nosql databases</v>
+        <v>software engineer, restful, react, sql, microservices, java, git, webpack, kanban, mysql, mongodb, programming, azure, front end, oracle, software development, npm, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
       </c>
       <c r="V13" t="str">
         <v>Full Stack Developer</v>
@@ -1448,12 +1454,12 @@
         <v>3.7</v>
       </c>
       <c r="AA13" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in front-end technologies and back-end frameworks | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with strong proficiency in Java and React.js | Design, develop, and maintain Java-based applications and microservices; collaborate in agile software development</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2026-01-10T14:13:36.642Z</v>
+        <v>2026-01-09T21:47:03.818Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1462,7 +1468,7 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-indore-3-to-8-years-090126931329</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-090126930803</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
@@ -1471,16 +1477,16 @@
         <v>Yes</v>
       </c>
       <c r="G14" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H14" t="str">
         <v>Yes</v>
       </c>
       <c r="I14" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J14" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K14" t="str">
         <v>External Apply</v>
@@ -1501,7 +1507,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q14" t="str">
-        <v>Indore</v>
+        <v>Chennai</v>
       </c>
       <c r="R14" t="str">
         <v>1 day ago</v>
@@ -1510,7 +1516,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U14" t="str">
-        <v>software engineer, front end, css, full stack development, version control, hibernate, javascript, web development frameworks, database management, java, git, postgresql, full stack, software solutions, mysql, web development, html, agile</v>
+        <v>software engineer, front end, application developer, css, restful, business processes, agile development, hibernate, javascript, sql, spring framework, database management, java, full stack, software solutions, construction, html, agile</v>
       </c>
       <c r="V14" t="str">
         <v>Full Stack Developer</v>
@@ -1528,12 +1534,12 @@
         <v>3.7</v>
       </c>
       <c r="AA14" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in web development frameworks like Spring and Hibernate | Develop custom software solutions, collaborate with cross-functional teams, and engage in continuous learning</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in front-end technologies | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2026-01-10T14:13:40.080Z</v>
+        <v>2026-01-09T21:47:07.081Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1542,7 +1548,7 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931192</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-indore-3-to-8-years-090126931329</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
@@ -1551,16 +1557,16 @@
         <v>Yes</v>
       </c>
       <c r="G15" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H15" t="str">
         <v>Yes</v>
       </c>
       <c r="I15" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J15" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K15" t="str">
         <v>External Apply</v>
@@ -1581,7 +1587,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q15" t="str">
-        <v>Hyderabad</v>
+        <v>Indore</v>
       </c>
       <c r="R15" t="str">
         <v>1 day ago</v>
@@ -1590,7 +1596,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U15" t="str">
-        <v>software engineer, rest, api development, restful, version control, user experience, sql, microservices, spring boot, database management, java, restful apis, git, microservices architecture, full stack, software solutions, agile, architecture</v>
+        <v>software engineer, front end, css, full stack development, version control, hibernate, javascript, web development frameworks, database management, java, git, postgresql, full stack, software solutions, mysql, web development, html, agile</v>
       </c>
       <c r="V15" t="str">
         <v>Full Stack Developer</v>
@@ -1608,12 +1614,12 @@
         <v>3.7</v>
       </c>
       <c r="AA15" t="str">
-        <v>Minimum 3 years of experience in Spring Boot; BTech, MTech, or MCA in IT, CSE, EEE, or ECE | Develop custom software solutions and RESTful APIs; Collaborate with cross-functional teams and stakeholders</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in web development frameworks like Spring and Hibernate | Develop custom software solutions, collaborate with cross-functional teams, and engage in continuous learning</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2026-01-10T14:13:43.386Z</v>
+        <v>2026-01-09T21:47:10.417Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1622,7 +1628,7 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126930327</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931192</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
@@ -1655,7 +1661,7 @@
         <v>Accenture</v>
       </c>
       <c r="O16" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P16" t="str">
         <v>Not Disclosed</v>
@@ -1670,7 +1676,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U16" t="str">
-        <v>software engineer, front end, css, full stack development, front end technologies, user experience, hibernate, javascript, nosql, sql, back end, database management, java, design, full stack, html, aws, nosql databases</v>
+        <v>software engineer, rest, api development, restful, version control, user experience, sql, microservices, spring boot, database management, java, restful apis, git, microservices architecture, full stack, software solutions, agile, architecture</v>
       </c>
       <c r="V16" t="str">
         <v>Full Stack Developer</v>
@@ -1688,12 +1694,12 @@
         <v>3.7</v>
       </c>
       <c r="AA16" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in front-end technologies | Lead design, build, and configuration of applications; collaborate with teams and ensure timely delivery</v>
+        <v>Minimum 3 years of experience in Spring Boot; BTech, MTech, or MCA in IT, CSE, EEE, or ECE | Develop custom software solutions and RESTful APIs; Collaborate with cross-functional teams and stakeholders</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2026-01-10T14:13:46.621Z</v>
+        <v>2026-01-09T21:47:13.653Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1702,7 +1708,7 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931441</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126930327</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
@@ -1735,7 +1741,7 @@
         <v>Accenture</v>
       </c>
       <c r="O17" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P17" t="str">
         <v>Not Disclosed</v>
@@ -1750,7 +1756,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U17" t="str">
-        <v>software engineer, front end, css, full stack development, version control, front end technologies, javascript, code quality, nosql, sql, spring boot, database management, java, git, full stack, software solutions, html, agile, nosql databases</v>
+        <v>software engineer, front end, css, full stack development, front end technologies, user experience, hibernate, javascript, nosql, sql, back end, database management, java, design, full stack, html, aws, nosql databases</v>
       </c>
       <c r="V17" t="str">
         <v>Full Stack Developer</v>
@@ -1768,12 +1774,12 @@
         <v>3.7</v>
       </c>
       <c r="AA17" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development; proficiency in front-end technologies and database management | Develop custom software solutions, collaborate with teams, conduct code reviews</v>
+        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in front-end technologies | Lead design, build, and configuration of applications; collaborate with teams and ensure timely delivery</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2026-01-10T14:13:49.940Z</v>
+        <v>2026-01-09T21:47:16.925Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1782,7 +1788,7 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-090126931749</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931441</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
@@ -1821,7 +1827,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q18" t="str">
-        <v>Gurugram</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R18" t="str">
         <v>1 day ago</v>
@@ -1830,7 +1836,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U18" t="str">
-        <v>software engineer, front end, application developer, restful, web services, version control, business processes, react, angular, database management, java, git, postgresql, full stack, software solutions, debugging, construction, mysql, agile</v>
+        <v>software engineer, front end, css, full stack development, version control, front end technologies, javascript, code quality, nosql, sql, spring boot, database management, java, git, full stack, software solutions, html, agile, nosql databases</v>
       </c>
       <c r="V18" t="str">
         <v>Full Stack Developer</v>
@@ -1848,12 +1854,12 @@
         <v>3.7</v>
       </c>
       <c r="AA18" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in RESTful web services and API integration | Develop custom software solutions, collaborate with teams, and ensure application performance</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development; proficiency in front-end technologies and database management | Develop custom software solutions, collaborate with teams, conduct code reviews</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2026-01-10T14:13:53.257Z</v>
+        <v>2026-01-09T21:47:20.178Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1862,7 +1868,7 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930810</v>
+        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-090126931749</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
@@ -1901,7 +1907,7 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q19" t="str">
-        <v>Bengaluru</v>
+        <v>Gurugram</v>
       </c>
       <c r="R19" t="str">
         <v>1 day ago</v>
@@ -1910,7 +1916,7 @@
         <v>Less than 10</v>
       </c>
       <c r="U19" t="str">
-        <v>software engineer, restful, full stack development, version control, database technologies, nosql, sql, web development frameworks, angular, java, git, api design, design, full stack, agile methodologies, software solutions, web development, agile</v>
+        <v>software engineer, front end, application developer, restful, web services, version control, business processes, react, angular, database management, java, git, postgresql, full stack, software solutions, debugging, construction, mysql, agile</v>
       </c>
       <c r="V19" t="str">
         <v>Full Stack Developer</v>
@@ -1928,12 +1934,12 @@
         <v>3.7</v>
       </c>
       <c r="AA19" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, and engage in code reviews</v>
+        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in RESTful web services and API integration | Develop custom software solutions, collaborate with teams, and ensure application performance</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2026-01-10T14:13:56.598Z</v>
+        <v>2026-01-09T21:47:23.460Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1987,7 +1993,7 @@
         <v>1 day ago</v>
       </c>
       <c r="S20" t="str">
-        <v>10</v>
+        <v>Less than 10</v>
       </c>
       <c r="U20" t="str">
         <v>software engineer, css, restful, react, sql, microservices, java, git, webpack, kanban, web development, azure, front end, oracle, software development, npm, javascript, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
@@ -2013,7 +2019,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2026-01-10T14:13:59.959Z</v>
+        <v>2026-01-09T21:47:26.839Z</v>
       </c>
       <c r="B21">
         <v>1</v>

</xml_diff>

<commit_message>
feat: Replace job cards with terminal logs in Job Engine
- Remove job cards UI and display terminal/command line instead
- Show live automation logs in terminal format
- Keep Applied/Skipped counters in status bar
- Terminal shows timestamp and colored logs (error=red, success=green, warning=yellow)
- Auto-scrolling terminal display
</commit_message>
<xml_diff>
--- a/naukri_results.xlsx
+++ b/naukri_results.xlsx
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-09T21:45:57.123Z</v>
+        <v>2026-01-11T12:35:19.667Z</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>1/20</v>
       </c>
       <c r="D2" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-micro-wings-mumbai-all-areas-2-to-7-years-180925000269</v>
+        <v>https://www.naukri.com/job-listings-java-full-stack-developers-infosoft-systems-pune-3-to-8-years-110126006457</v>
       </c>
       <c r="E2" t="str">
         <v>Yes</v>
@@ -505,49 +505,49 @@
         <v>Yes</v>
       </c>
       <c r="G2" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H2" t="str">
         <v>Yes</v>
       </c>
       <c r="I2" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J2" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K2" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L2" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M2" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Java Full Stack Developers</v>
       </c>
       <c r="N2" t="str">
-        <v>Micro Wings</v>
+        <v>Infosoft Systems</v>
       </c>
       <c r="O2" t="str">
-        <v>2 - 7 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P2" t="str">
-        <v>3-6 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q2" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Pune</v>
       </c>
       <c r="R2" t="str">
-        <v>1 day ago</v>
+        <v>Few hours ago</v>
       </c>
       <c r="S2" t="str">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T2" t="str">
         <v>100+</v>
       </c>
       <c r="U2" t="str">
-        <v>Java, Hibernate, Spring Boot, Java Fullstack, Angular, Debugging Skills, Cross Functional Coordination, Maven, Spring Mvc, SOAP UI, Postgresql, HTML, Oops Programming, JIRA, Microservices, JUnit, JSP Servlets, Postman Tool, Java Development, Restful Web Api Development</v>
+        <v>Java, Spring Boot, Java Fullstack, Microservices, Flutter, Mobile Development, Web Application Development, Angular, Mobile Application Development, SQL, Android Application Development, Rest, MySQL, Javascript, Web Application, React.Js, Android Studio, Web Development, Dart</v>
       </c>
       <c r="V2" t="str">
         <v>Full Stack Developer</v>
@@ -562,12 +562,12 @@
         <v>Software Development</v>
       </c>
       <c r="AA2" t="str">
-        <v>Proficient in Java, Spring Boot, Hibernate, Angular, and SQL | Develop and integrate SOAP/REST services, manage transactions, and perform debugging</v>
+        <v>5-6 years experience as a Java Full Stack Developer; proficiency in Java, Spring Boot, Hibernate, and front-end technologies like Angular or React | Design and maintain web and mobile applications; develop RESTful APIs; perform unit testing and debugging</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2026-01-09T21:46:00.411Z</v>
+        <v>2026-01-11T12:35:48.959Z</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -576,7 +576,7 @@
         <v>2/20</v>
       </c>
       <c r="D3" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-opus-pune-2-to-5-years-080126504723</v>
+        <v>https://www.naukri.com/job-listings-manager-it-development-full-stack-trafigura-mumbai-0-to-3-years-100126000786</v>
       </c>
       <c r="E3" t="str">
         <v>Yes</v>
@@ -588,52 +588,49 @@
         <v>Yes</v>
       </c>
       <c r="H3" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I3" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J3" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K3" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L3" t="str">
         <v>Skipped</v>
       </c>
       <c r="M3" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Manager - IT Development Full Stack</v>
       </c>
       <c r="N3" t="str">
-        <v>Opus Technosoft</v>
+        <v>Trafigura</v>
       </c>
       <c r="O3" t="str">
-        <v>2 - 5 years</v>
+        <v>0 - 3 years</v>
       </c>
       <c r="P3" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q3" t="str">
-        <v>Pune</v>
+        <v>Mumbai</v>
       </c>
       <c r="R3" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S3" t="str">
-        <v>1</v>
-      </c>
-      <c r="T3" t="str">
         <v>100+</v>
       </c>
       <c r="U3" t="str">
-        <v>SAN, Front end, French, GIT, Shaping, MySQL, Javascript, HTML, payment solutions, Monitoring</v>
+        <v>continuous integration, aws iam, solution development, cloud technologies, microservices, react.js, java, ui, lean, design, digital, cd, python, development, gui testing, technology, spring boot, angular, node.js, re, application, lambda expressions, delivery management, web technologies, agile, aws</v>
       </c>
       <c r="V3" t="str">
-        <v>Full Stack Developer</v>
+        <v>Head - Engineering</v>
       </c>
       <c r="W3" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Oil &amp; Gas</v>
       </c>
       <c r="X3" t="str">
         <v>Full Time, Permanent</v>
@@ -641,13 +638,16 @@
       <c r="Y3" t="str">
         <v>Software Development</v>
       </c>
+      <c r="Z3" t="str">
+        <v>3.2</v>
+      </c>
       <c r="AA3" t="str">
-        <v>Required Skills &amp; Experience . Strong proficiency in Java and Angular | Experience with version control systems (Git and BitBucket) | Experience with Postman for API testing and JUnit for unit testing . Hands-on experience with Keycloak (authentication &amp; authorization) and Kibana (log monitoring &amp; analytics) | Experience with AWS cloud services</v>
+        <v>5+ years experience in digital product design and development; knowledge of Cloud Technologies and Web technologies (Angular, ReactJS, NodeJs, JAVA Spring Boot) | Assess existing processes, develop user stories, consult on product design, and monitor product performance</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2026-01-09T21:46:03.678Z</v>
+        <v>2026-01-11T12:35:52.374Z</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -656,7 +656,7 @@
         <v>3/20</v>
       </c>
       <c r="D4" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930984</v>
+        <v>https://www.naukri.com/job-listings-full-stack-engineer-full-time-exaflair-technologies-mohali-chandigarh-zirakpur-1-to-3-years-110126007520</v>
       </c>
       <c r="E4" t="str">
         <v>Yes</v>
@@ -665,49 +665,52 @@
         <v>Yes</v>
       </c>
       <c r="G4" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H4" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I4" t="str">
-        <v>4/undefined</v>
+        <v>2/undefined</v>
       </c>
       <c r="J4" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K4" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L4" t="str">
         <v>Skipped</v>
       </c>
       <c r="M4" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Full Stack Engineer(full-time)</v>
       </c>
       <c r="N4" t="str">
-        <v>Accenture</v>
+        <v>Exaflair Technologies</v>
       </c>
       <c r="O4" t="str">
-        <v>2 - 5 years</v>
+        <v>1 - 3 years</v>
       </c>
       <c r="P4" t="str">
-        <v>Not Disclosed</v>
+        <v>4-6 Lacs P.A.</v>
       </c>
       <c r="Q4" t="str">
-        <v>Bengaluru</v>
+        <v>Mohali</v>
       </c>
       <c r="R4" t="str">
-        <v>1 day ago</v>
+        <v>Just now</v>
       </c>
       <c r="S4" t="str">
+        <v>1</v>
+      </c>
+      <c r="T4" t="str">
         <v>Less than 10</v>
       </c>
       <c r="U4" t="str">
-        <v>software engineer, github, restful, api gateway, html5, full stack developer, redis, nosql, sql, microservices, docker, angular, spring boot, java, restful apis, git, postgresql, full stack, mysql, typescript, agile, mongodb, css3, architecture</v>
+        <v>Typescript, SQL/NoSQL/PostgreSQL, Node.Js, React.Js, Nextjs, Express, Javascript, Github Actions, Tailwind Css, Vite</v>
       </c>
       <c r="V4" t="str">
-        <v>Blockchain Quality Assurance Engineer</v>
+        <v>Application Engineer</v>
       </c>
       <c r="W4" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -716,18 +719,15 @@
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y4" t="str">
-        <v>Quality Assurance and Testing</v>
-      </c>
-      <c r="Z4" t="str">
-        <v>3.7</v>
+        <v>Engineering</v>
       </c>
       <c r="AA4" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with expertise in Angular and microservices | Develop custom software solutions, collaborate with cross-functional teams, and ensure high-quality performance</v>
+        <v>Bachelor's degree in Computer Science or related field; 1-3 years of full-stack development experience; strong skills in TypeScript/JavaScript, Next.js, and React | Develop and maintain full-stack features; build responsive frontend interfaces; implement backend logic and APIs | Competitive compensation based on experience and impact</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2026-01-09T21:46:06.979Z</v>
+        <v>2026-01-11T12:35:55.626Z</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -736,13 +736,13 @@
         <v>4/20</v>
       </c>
       <c r="D5" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-grid-dynamics-bengaluru-3-to-5-years-080126501444</v>
+        <v>https://www.naukri.com/job-listings-senior-software-engineer-java-great-west-global-business-services-bengaluru-3-to-8-years-110126005561</v>
       </c>
       <c r="E5" t="str">
         <v>Yes</v>
       </c>
       <c r="F5" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G5" t="str">
         <v>Yes</v>
@@ -751,25 +751,25 @@
         <v>Yes</v>
       </c>
       <c r="I5" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J5" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K5" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L5" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M5" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Senior Software Engineer - Java</v>
       </c>
       <c r="N5" t="str">
-        <v>Grid Dynamics</v>
+        <v>Empower</v>
       </c>
       <c r="O5" t="str">
-        <v>3 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P5" t="str">
         <v>Not Disclosed</v>
@@ -778,22 +778,19 @@
         <v>Bengaluru</v>
       </c>
       <c r="R5" t="str">
-        <v>1 day ago</v>
+        <v>Today</v>
       </c>
       <c r="S5" t="str">
-        <v>1</v>
-      </c>
-      <c r="T5" t="str">
-        <v>50+</v>
+        <v>100+</v>
       </c>
       <c r="U5" t="str">
-        <v>Backend, Db2, XML, MySQL, Data structures, Data processing, JSON, Oracle, Financial services</v>
+        <v>continuous integration, kubernetes, analytical, concurrent, ci/cd, sql, plsql, database development, docker, spring, java, postgresql, multithreading, mysql, boot, communication skills, cd, rest, oracle, version control, maven, orm, spring boot framework, relational databases, gradle, scrum, agile, aws</v>
       </c>
       <c r="V5" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W5" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Financial Services</v>
       </c>
       <c r="X5" t="str">
         <v>Full Time, Permanent</v>
@@ -802,15 +799,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z5" t="str">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="AA5" t="str">
-        <v/>
+        <v>5+ years of back-end engineering experience in Java, Spring, and database development | Design, develop, and troubleshoot software features in an Agile/Scrum environment; lead coding efforts and participate in architectural discussions</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2026-01-09T21:46:10.282Z</v>
+        <v>2026-01-11T12:36:24.187Z</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -819,7 +816,7 @@
         <v>5/20</v>
       </c>
       <c r="D6" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-capital-business-systems-prayagraj-3-to-7-years-090126011977</v>
+        <v>https://www.naukri.com/job-listings-it-full-stack-developer-rad-trafigura-mumbai-0-to-3-years-100126000785</v>
       </c>
       <c r="E6" t="str">
         <v>Yes</v>
@@ -828,10 +825,10 @@
         <v>Yes</v>
       </c>
       <c r="G6" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="H6" t="str">
         <v>No</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Yes</v>
       </c>
       <c r="I6" t="str">
         <v>3/undefined</v>
@@ -846,37 +843,34 @@
         <v>Skipped</v>
       </c>
       <c r="M6" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>IT Full Stack Developer - RAD</v>
       </c>
       <c r="N6" t="str">
-        <v>Capital Business Systems</v>
+        <v>Trafigura</v>
       </c>
       <c r="O6" t="str">
-        <v>3 - 7 years</v>
+        <v>0 - 3 years</v>
       </c>
       <c r="P6" t="str">
-        <v>5-10 Lacs P.A.</v>
+        <v>Not Disclosed</v>
       </c>
       <c r="Q6" t="str">
-        <v>Prayagraj</v>
+        <v>Mumbai</v>
       </c>
       <c r="R6" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S6" t="str">
-        <v>1</v>
-      </c>
-      <c r="T6" t="str">
         <v>100+</v>
       </c>
       <c r="U6" t="str">
-        <v>Java, Angular, Hibernate, Postgresql, MySQL, Spring Boot, J2Ee, Java Fullstack, Spring, Microservices</v>
+        <v>server, continuous integration, kubernetes, css, analytical, ci/cd, react.js, devops, asp.net, jenkins, end, typescript, api, graphql, communication skills, architecture, c#, cd, side, development, python, oracle, microsoft azure, javascript, sql server, angular, .net, scrum, gitlab, front, agile, aws, asp</v>
       </c>
       <c r="V6" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W6" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Oil &amp; Gas</v>
       </c>
       <c r="X6" t="str">
         <v>Full Time, Permanent</v>
@@ -885,15 +879,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z6" t="str">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="AA6" t="str">
-        <v>Full-stack developer with hands-on experience in Java (J2EE, Spring Boot, Hibernate) and modern front-end frameworks like Angular or React | Develop front-end interfaces, build back-end services, design RESTful APIs, manage databases, and deploy applications using DevOps tools</v>
+        <v>Bachelor's degree in Computer Science or related field with 8+ years of full stack development experience | Manage end-to-end development lifecycle, collaborate on technical design, and resolve high-severity issues</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2026-01-09T21:46:13.574Z</v>
+        <v>2026-01-11T12:36:27.520Z</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -902,7 +896,7 @@
         <v>6/20</v>
       </c>
       <c r="D7" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-3i-infotech-mumbai-all-areas-2-to-7-years-080126016500</v>
+        <v>https://www.naukri.com/job-listings-software-engineer-kayhan-space-bengaluru-2-to-5-years-110126005505</v>
       </c>
       <c r="E7" t="str">
         <v>Yes</v>
@@ -911,49 +905,49 @@
         <v>Yes</v>
       </c>
       <c r="G7" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H7" t="str">
         <v>Yes</v>
       </c>
       <c r="I7" t="str">
-        <v>3/undefined</v>
+        <v>4/undefined</v>
       </c>
       <c r="J7" t="str">
-        <v>Poor Match</v>
+        <v>Good Match</v>
       </c>
       <c r="K7" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L7" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M7" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Software Engineer</v>
       </c>
       <c r="N7" t="str">
-        <v>3i Infotech</v>
+        <v>Kayhan Space</v>
       </c>
       <c r="O7" t="str">
-        <v>2 - 7 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P7" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q7" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R7" t="str">
-        <v>1 day ago</v>
+        <v>Today</v>
       </c>
       <c r="S7" t="str">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="T7" t="str">
         <v>100+</v>
       </c>
       <c r="U7" t="str">
-        <v>React.Js, Angular, Java Spring Boot, HTML, Java Fullstack, AWS</v>
+        <v>C, or high-volume timeseries data processing, astrodynamics, React.Js, Frontend Web Development, C++, Rust, Postgresql, MCP applications, Typescript, agentic workflows, containerized software deployment and Kubernetes, physics, LLM integrations, statistical analysis, Nextjs, AWS</v>
       </c>
       <c r="V7" t="str">
         <v>Software Development - Other</v>
@@ -967,16 +961,13 @@
       <c r="Y7" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z7" t="str">
-        <v>3.4</v>
-      </c>
       <c r="AA7" t="str">
-        <v>Bachelor's degree in Computer Science or related field with 3+ years of experience in Java Full Stack Development | Design, develop, and maintain full-stack web applications using Java and modern frameworks; develop backend services and build responsive frontend interfaces</v>
+        <v>Bachelor's degree in Computer Science, 2+ years in software development, strong Python and PostgreSQL skills | Design and maintain features for Satcat.com, build internal automation and dashboards, advocate for user experience excellence</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2026-01-09T21:46:16.919Z</v>
+        <v>2026-01-11T12:36:58.765Z</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -985,13 +976,13 @@
         <v>7/20</v>
       </c>
       <c r="D8" t="str">
-        <v>https://www.naukri.com/job-listings-java-full-stack-developer-3i-infotech-hyderabad-mumbai-all-areas-3-to-8-years-080126010394</v>
+        <v>https://www.naukri.com/job-listings-multiple-openings-java-linux-android-full-stack-ds-i-testing-hirex-consultancy-services-hyderabad-pune-bengaluru-3-to-8-years-110126006910</v>
       </c>
       <c r="E8" t="str">
         <v>Yes</v>
       </c>
       <c r="F8" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G8" t="str">
         <v>Yes</v>
@@ -1000,46 +991,46 @@
         <v>Yes</v>
       </c>
       <c r="I8" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J8" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K8" t="str">
         <v>Direct Apply</v>
       </c>
       <c r="L8" t="str">
-        <v>Applied</v>
+        <v>Skipped</v>
       </c>
       <c r="M8" t="str">
-        <v>Java Full Stack Developer</v>
+        <v>Multiple Openings | Java | Linux | Android | Full Stack | DS I Testing</v>
       </c>
       <c r="N8" t="str">
-        <v>3i Infotech</v>
+        <v>HiREx Consultancy Services</v>
       </c>
       <c r="O8" t="str">
         <v>3 - 8 years</v>
       </c>
       <c r="P8" t="str">
-        <v>13-23 Lacs P.A.</v>
+        <v>8-18 Lacs P.A.</v>
       </c>
       <c r="Q8" t="str">
-        <v>Mumbai (All Areas)</v>
+        <v>Pune</v>
       </c>
       <c r="R8" t="str">
-        <v>1 day ago</v>
+        <v>Few hours ago</v>
       </c>
       <c r="S8" t="str">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="T8" t="str">
-        <v>100+</v>
+        <v>50+</v>
       </c>
       <c r="U8" t="str">
-        <v>Java, Spring Boot, API, React.Js, Angular, SQL</v>
+        <v>C++, Middleware, Linux, Fullstack Development, Automation Testing, Java, C, J2Ee, Mobile Application Development, Android, Application Development, Android Application Development, application, Frontend Development, Middleware Technologies, Linux Kernel</v>
       </c>
       <c r="V8" t="str">
-        <v>Full Stack Developer</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W8" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1050,16 +1041,13 @@
       <c r="Y8" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z8" t="str">
-        <v>3.4</v>
-      </c>
       <c r="AA8" t="str">
-        <v>Bachelor’s degree in Computer Science or Engineering; strong proficiency in Java, Spring Boot, and modern frontend frameworks like Angular or React | Design, develop, and maintain full stack web applications; develop backend services and RESTful APIs; build responsive UI components</v>
+        <v>Experienced professionals in technology domains with skills in Java, Linux, and Middleware | Work on cutting-edge technologies and large-scale enterprise applications across various roles</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2026-01-09T21:46:46.923Z</v>
+        <v>2026-01-11T12:37:02.104Z</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1068,7 +1056,7 @@
         <v>8/20</v>
       </c>
       <c r="D9" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126931488</v>
+        <v>https://www.naukri.com/job-listings-software-developer-react-native-chola-ms-chennai-3-to-7-years-110126005675</v>
       </c>
       <c r="E9" t="str">
         <v>Yes</v>
@@ -1089,40 +1077,43 @@
         <v>Good Match</v>
       </c>
       <c r="K9" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L9" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M9" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Software Developer - React Native</v>
       </c>
       <c r="N9" t="str">
-        <v>Accenture</v>
+        <v>Chola MS</v>
       </c>
       <c r="O9" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P9" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q9" t="str">
-        <v>Hyderabad</v>
+        <v>Chennai</v>
       </c>
       <c r="R9" t="str">
-        <v>1 day ago</v>
+        <v>Today</v>
       </c>
       <c r="S9" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T9" t="str">
+        <v>100+</v>
       </c>
       <c r="U9" t="str">
-        <v>software engineer, front end, css, api development, restful, full stack development, version control, front end technologies, javascript, spring boot, java, git, design, full stack, software solutions, html, agile</v>
+        <v>React Native, Native, React Native Js</v>
       </c>
       <c r="V9" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W9" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Insurance</v>
       </c>
       <c r="X9" t="str">
         <v>Full Time, Permanent</v>
@@ -1131,15 +1122,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z9" t="str">
-        <v>3.7</v>
+        <v>4.0</v>
       </c>
       <c r="AA9" t="str">
-        <v>Minimum 2 years experience in Java Full Stack Development; proficiency in front-end technologies and RESTful API integration | Develop custom software solutions, collaborate with teams, and assist in documentation</v>
+        <v>Bachelor's degree in Computer Science; 4-6 years of experience in React Native development; strong problem-solving skills | Design, develop, and maintain mobile and web applications; troubleshoot technical issues; collaborate with team members</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2026-01-09T21:46:50.246Z</v>
+        <v>2026-01-11T12:37:32.245Z</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1148,7 +1139,7 @@
         <v>9/20</v>
       </c>
       <c r="D10" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-2-to-5-years-090126930110</v>
+        <v>https://www.naukri.com/job-listings-software-java-developer-creative-hands-hr-hyderabad-chennai-bengaluru-0-to-5-years-100126012778</v>
       </c>
       <c r="E10" t="str">
         <v>Yes</v>
@@ -1169,37 +1160,40 @@
         <v>Good Match</v>
       </c>
       <c r="K10" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L10" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M10" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Software-Java Developer</v>
       </c>
       <c r="N10" t="str">
-        <v>Accenture</v>
+        <v>Creative Hands HR</v>
       </c>
       <c r="O10" t="str">
-        <v>2 - 5 years</v>
+        <v>0 - 5 years</v>
       </c>
       <c r="P10" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q10" t="str">
-        <v>Bengaluru</v>
+        <v>Chennai</v>
       </c>
       <c r="R10" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S10" t="str">
-        <v>Less than 10</v>
+        <v>100</v>
+      </c>
+      <c r="T10" t="str">
+        <v>100+</v>
       </c>
       <c r="U10" t="str">
-        <v>software engineer, front end, kubernetes, css, api development, javascript, nosql, sql, docker, angular, spring boot, back end, database management, java, git, oops, full stack, web development, typescript, agile, aws, nosql databases</v>
+        <v>Java, Multithreading, Docker, Spring Boot, Collections, AWS, Microservices, Restful Web Api Development</v>
       </c>
       <c r="V10" t="str">
-        <v>Full Stack Developer</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W10" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1210,16 +1204,13 @@
       <c r="Y10" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z10" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA10" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern frameworks like Spring and Angular | Design, develop, and maintain web applications; collaborate with teams to deliver scalable solutions</v>
+        <v>Proficiency in Java and Spring Boot, strong understanding of multithreading and collections, experience with microservices and Docker | Develop and implement RESTful APIs, manage Docker environments, apply microservices design patterns</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2026-01-09T21:46:53.561Z</v>
+        <v>2026-01-11T12:37:44.555Z</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1228,7 +1219,7 @@
         <v>10/20</v>
       </c>
       <c r="D11" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-2-to-5-years-090126931461</v>
+        <v>https://www.naukri.com/job-listings-sr-engineer-automation-great-west-global-business-services-bengaluru-3-to-8-years-110126004675</v>
       </c>
       <c r="E11" t="str">
         <v>Yes</v>
@@ -1249,57 +1240,57 @@
         <v>Good Match</v>
       </c>
       <c r="K11" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L11" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M11" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Sr Engineer Automation</v>
       </c>
       <c r="N11" t="str">
-        <v>Accenture</v>
+        <v>Empower</v>
       </c>
       <c r="O11" t="str">
-        <v>2 - 5 years</v>
+        <v>3 - 8 years</v>
       </c>
       <c r="P11" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q11" t="str">
-        <v>Pune</v>
+        <v>Bengaluru</v>
       </c>
       <c r="R11" t="str">
-        <v>1 day ago</v>
+        <v>Today</v>
       </c>
       <c r="S11" t="str">
-        <v>Less than 10</v>
+        <v>50+</v>
       </c>
       <c r="U11" t="str">
-        <v>software engineer, restful, software development, full stack development, version control, nosql, sql, angular, database management, java, git, web frameworks, api design, design, full stack, software solutions, agile, nosql databases</v>
+        <v>kubernetes, interpersonal skills, ssh, ssl, apache tomcat, docker, ansible, java, automation tools, apache, jboss, aws cloud, linux, jenkins, j2ee, debugging, shell scripting, perl, solaris, programming, communication skills, python, c, ftp, ant, weblogic, puppet, teamwork, troubleshooting, gitlab, aws, unix</v>
       </c>
       <c r="V11" t="str">
-        <v>Full Stack Developer</v>
+        <v>Site Reliability Engineer</v>
       </c>
       <c r="W11" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Financial Services</v>
       </c>
       <c r="X11" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y11" t="str">
-        <v>Software Development</v>
+        <v>DevOps</v>
       </c>
       <c r="Z11" t="str">
-        <v>3.7</v>
+        <v>4.0</v>
       </c>
       <c r="AA11" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in modern web frameworks like Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>B.S. in Computer Information Systems or Engineering; 4-6 years programming experience; 2+ years AWS cloud &amp; automation tools experience | Convince organization on architecture best practices; Create automated build infrastructure; Drive debugging and troubleshooting operations</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2026-01-09T21:46:57.181Z</v>
+        <v>2026-01-11T12:38:13.112Z</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1308,13 +1299,13 @@
         <v>11/20</v>
       </c>
       <c r="D12" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-2-to-5-years-090126930317</v>
+        <v>https://www.naukri.com/job-listings-asp-net-developer-full-stack-guntur-hyderabad-bookxpert-guntur-hyderabad-2-to-5-years-271124013249</v>
       </c>
       <c r="E12" t="str">
         <v>Yes</v>
       </c>
       <c r="F12" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G12" t="str">
         <v>Yes</v>
@@ -1323,22 +1314,22 @@
         <v>Yes</v>
       </c>
       <c r="I12" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J12" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K12" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L12" t="str">
         <v>Skipped</v>
       </c>
       <c r="M12" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Asp.Net Developer- Full Stack- Guntur/Hyderabad</v>
       </c>
       <c r="N12" t="str">
-        <v>Accenture</v>
+        <v>Bookxpert</v>
       </c>
       <c r="O12" t="str">
         <v>2 - 5 years</v>
@@ -1347,22 +1338,25 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q12" t="str">
-        <v>Chennai</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R12" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S12" t="str">
-        <v>Less than 10</v>
+        <v>5</v>
+      </c>
+      <c r="T12" t="str">
+        <v>100+</v>
       </c>
       <c r="U12" t="str">
-        <v>software engineer, restful, software development, nosql, sql, web development frameworks, angular, database management, java, git, api design, full stack, agile methodologies, software solutions, web development, agile, nosql databases</v>
+        <v>C#, My SQL/MS SQL Server Database, Asp.Net Web Api, Team Player, Net Fullstack, Analytical Skills, Planning Skills, Asp.Net Core Mvc, VB, Leadership Skills, Presentation Skills, Communication Skills, Coding, Javascript, React.Js</v>
       </c>
       <c r="V12" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W12" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Accounting / Auditing</v>
       </c>
       <c r="X12" t="str">
         <v>Full Time, Permanent</v>
@@ -1371,15 +1365,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z12" t="str">
-        <v>3.7</v>
+        <v>4.3</v>
       </c>
       <c r="AA12" t="str">
-        <v>Minimum 7.5 years of experience in Java Full Stack Development with proficiency in Spring and Angular | Develop custom software solutions, collaborate with teams, mentor junior members, and improve development processes</v>
+        <v>Strong hands-on experience with ASP.NET MVC/Core and C#, proficiency in JavaScript (ES6+), React.js, and TypeScript | Design, develop, and maintain applications; build front-end components; develop RESTful APIs; collaborate with teams; perform debugging and code reviews | Competitive salary and professional development opportunities</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2026-01-09T21:47:00.548Z</v>
+        <v>2026-01-11T12:38:16.420Z</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1388,7 +1382,7 @@
         <v>12/20</v>
       </c>
       <c r="D13" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930328</v>
+        <v>https://www.naukri.com/job-listings-senior-software-engineer-tapza-technologies-warangal-hyderabad-3-to-7-years-100126036500</v>
       </c>
       <c r="E13" t="str">
         <v>Yes</v>
@@ -1409,37 +1403,40 @@
         <v>Good Match</v>
       </c>
       <c r="K13" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L13" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M13" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Senior Software Engineer</v>
       </c>
       <c r="N13" t="str">
-        <v>Accenture</v>
+        <v>Tapza Technologies</v>
       </c>
       <c r="O13" t="str">
-        <v>3 - 8 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P13" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q13" t="str">
-        <v>Bengaluru</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R13" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S13" t="str">
-        <v>Less than 10</v>
+        <v>2</v>
+      </c>
+      <c r="T13" t="str">
+        <v>100+</v>
       </c>
       <c r="U13" t="str">
-        <v>software engineer, restful, react, sql, microservices, java, git, webpack, kanban, mysql, mongodb, programming, azure, front end, oracle, software development, npm, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
+        <v>Node.Js, Javascript, Postgresql, Ci/Cd, Devops, Microservices, Laravel Php, Docker, Typescript, PHP, MongoDB, React.Js, AWS, Nestjs, Python</v>
       </c>
       <c r="V13" t="str">
-        <v>Full Stack Developer</v>
+        <v>Back End Developer</v>
       </c>
       <c r="W13" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1451,15 +1448,15 @@
         <v>Software Development</v>
       </c>
       <c r="Z13" t="str">
-        <v>3.7</v>
+        <v>4.8</v>
       </c>
       <c r="AA13" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with strong proficiency in Java and React.js | Design, develop, and maintain Java-based applications and microservices; collaborate in agile software development</v>
+        <v>3 to 7+ years of backend-focused software engineering experience with strong fundamentals in system design and data modeling | Design and build scalable backend systems, translate product requirements into system designs, and mentor junior engineers | Competitive compensation and meaningful ESOP as part of the founding team</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2026-01-09T21:47:03.818Z</v>
+        <v>2026-01-11T12:38:45.781Z</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1468,7 +1465,7 @@
         <v>13/20</v>
       </c>
       <c r="D14" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-chennai-3-to-8-years-090126930803</v>
+        <v>https://www.naukri.com/job-listings-java-back-end-developer-3-to-10-years-erudio-technologies-chennai-3-to-8-years-110126007341</v>
       </c>
       <c r="E14" t="str">
         <v>Yes</v>
@@ -1489,37 +1486,40 @@
         <v>Good Match</v>
       </c>
       <c r="K14" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L14" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M14" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Java Back End Developer (3 To 10 years)</v>
       </c>
       <c r="N14" t="str">
-        <v>Accenture</v>
+        <v>Erudio Technologies</v>
       </c>
       <c r="O14" t="str">
         <v>3 - 8 years</v>
       </c>
       <c r="P14" t="str">
-        <v>Not Disclosed</v>
+        <v>8-18 Lacs P.A.</v>
       </c>
       <c r="Q14" t="str">
         <v>Chennai</v>
       </c>
       <c r="R14" t="str">
-        <v>1 day ago</v>
+        <v>Just now</v>
       </c>
       <c r="S14" t="str">
-        <v>Less than 10</v>
+        <v>50</v>
+      </c>
+      <c r="T14" t="str">
+        <v>49</v>
       </c>
       <c r="U14" t="str">
-        <v>software engineer, front end, application developer, css, restful, business processes, agile development, hibernate, javascript, sql, spring framework, database management, java, full stack, software solutions, construction, html, agile</v>
+        <v>Javascript, Spring Boot, Microservices, Java, Hibernate, HTML, Java Fullstack, React.Js, Angular, SQL, Python</v>
       </c>
       <c r="V14" t="str">
-        <v>Full Stack Developer</v>
+        <v>Back End Developer</v>
       </c>
       <c r="W14" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1530,16 +1530,13 @@
       <c r="Y14" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z14" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA14" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in front-end technologies | Develop custom software solutions, engage in design and code reviews, and assist in documentation</v>
+        <v>Skilled Java Backend Developer with expertise in Java (8+), Spring Boot, and microservices architecture | Develop and maintain backend applications, design scalable microservices, and integrate RESTful APIs</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2026-01-09T21:47:07.081Z</v>
+        <v>2026-01-11T12:38:58.085Z</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1548,16 +1545,16 @@
         <v>14/20</v>
       </c>
       <c r="D15" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-indore-3-to-8-years-090126931329</v>
+        <v>https://www.naukri.com/job-listings-java-developers-openings-vedamcloud-technologies-bangalore-bengaluru-0-to-5-years-100126011241</v>
       </c>
       <c r="E15" t="str">
         <v>Yes</v>
       </c>
       <c r="F15" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G15" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H15" t="str">
         <v>Yes</v>
@@ -1569,34 +1566,37 @@
         <v>Poor Match</v>
       </c>
       <c r="K15" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L15" t="str">
         <v>Skipped</v>
       </c>
       <c r="M15" t="str">
-        <v>Custom Software Engineer</v>
+        <v>JAVA Developers Job Openings</v>
       </c>
       <c r="N15" t="str">
-        <v>Accenture</v>
+        <v>Vedamcloud Technologies</v>
       </c>
       <c r="O15" t="str">
-        <v>3 - 8 years</v>
+        <v>0 - 5 years</v>
       </c>
       <c r="P15" t="str">
-        <v>Not Disclosed</v>
+        <v>5-15 Lacs P.A.</v>
       </c>
       <c r="Q15" t="str">
-        <v>Indore</v>
+        <v>Bangalore/Bengaluru</v>
       </c>
       <c r="R15" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S15" t="str">
-        <v>Less than 10</v>
+        <v>6</v>
+      </c>
+      <c r="T15" t="str">
+        <v>100+</v>
       </c>
       <c r="U15" t="str">
-        <v>software engineer, front end, css, full stack development, version control, hibernate, javascript, web development frameworks, database management, java, git, postgresql, full stack, software solutions, mysql, web development, html, agile</v>
+        <v>SQL, Java, Oracle Apps Technical, Rice Components, Oracle Database, Java Programming, Java Web Services, J2Ee, Core Java Programming, J2Ee Development, JSP Servlets, XML Publisher Reports, Java Development, PLSQL, JDBC, Oracle, Core Java Development</v>
       </c>
       <c r="V15" t="str">
         <v>Full Stack Developer</v>
@@ -1610,16 +1610,13 @@
       <c r="Y15" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z15" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA15" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in web development frameworks like Spring and Hibernate | Develop custom software solutions, collaborate with cross-functional teams, and engage in continuous learning</v>
+        <v>Freshers with knowledge of Java and OOPS concepts | Work as a JAVA Developer for Indian clients</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2026-01-09T21:47:10.417Z</v>
+        <v>2026-01-11T12:39:01.342Z</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1628,7 +1625,7 @@
         <v>15/20</v>
       </c>
       <c r="D16" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931192</v>
+        <v>https://www.naukri.com/job-listings-ai-ml-engineer-worldclass-tech-talent-bengaluru-3-to-6-years-271025020222</v>
       </c>
       <c r="E16" t="str">
         <v>Yes</v>
@@ -1649,37 +1646,40 @@
         <v>Good Match</v>
       </c>
       <c r="K16" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L16" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M16" t="str">
-        <v>Custom Software Engineer</v>
+        <v>AI/ML Engineer</v>
       </c>
       <c r="N16" t="str">
-        <v>Accenture</v>
+        <v>Worldclass Tech Talent Pvt Ltd</v>
       </c>
       <c r="O16" t="str">
-        <v>3 - 8 years</v>
+        <v>3 - 6 years</v>
       </c>
       <c r="P16" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q16" t="str">
-        <v>Hyderabad</v>
+        <v>Bengaluru( BTM 2nd Stage )</v>
       </c>
       <c r="R16" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S16" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T16" t="str">
+        <v>50+</v>
       </c>
       <c r="U16" t="str">
-        <v>software engineer, rest, api development, restful, version control, user experience, sql, microservices, spring boot, database management, java, restful apis, git, microservices architecture, full stack, software solutions, agile, architecture</v>
+        <v>Python, Docker, PostgreSQL, LangChain, FastAPI/Flask, Microservices</v>
       </c>
       <c r="V16" t="str">
-        <v>Full Stack Developer</v>
+        <v>Data Platform Engineer</v>
       </c>
       <c r="W16" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1690,16 +1690,13 @@
       <c r="Y16" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z16" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA16" t="str">
-        <v>Minimum 3 years of experience in Spring Boot; BTech, MTech, or MCA in IT, CSE, EEE, or ECE | Develop custom software solutions and RESTful APIs; Collaborate with cross-functional teams and stakeholders</v>
+        <v>3+ years of experience in AI/ML with skills in Python, FastAPI/Flask, and LangChain | Develop and integrate backend solutions using Python and various databases</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2026-01-09T21:47:13.653Z</v>
+        <v>2026-01-11T12:39:13.640Z</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1708,7 +1705,7 @@
         <v>16/20</v>
       </c>
       <c r="D17" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-2-to-5-years-090126930327</v>
+        <v>https://www.naukri.com/job-listings-dot-net-developer-clama-india-pvt-ltd-thane-2-to-4-years-100126017165</v>
       </c>
       <c r="E17" t="str">
         <v>Yes</v>
@@ -1717,49 +1714,52 @@
         <v>Yes</v>
       </c>
       <c r="G17" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H17" t="str">
         <v>Yes</v>
       </c>
       <c r="I17" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J17" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K17" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L17" t="str">
         <v>Skipped</v>
       </c>
       <c r="M17" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Dot Net Developer</v>
       </c>
       <c r="N17" t="str">
-        <v>Accenture</v>
+        <v>Clama India Pvt. Ltd.</v>
       </c>
       <c r="O17" t="str">
-        <v>2 - 5 years</v>
+        <v>2 - 4 years</v>
       </c>
       <c r="P17" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q17" t="str">
-        <v>Hyderabad</v>
+        <v>Thane</v>
       </c>
       <c r="R17" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S17" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T17" t="str">
+        <v>50+</v>
       </c>
       <c r="U17" t="str">
-        <v>software engineer, front end, css, full stack development, front end technologies, user experience, hibernate, javascript, nosql, sql, back end, database management, java, design, full stack, html, aws, nosql databases</v>
+        <v>React.Js, Angular, Typescript, Javascript, Html/Css</v>
       </c>
       <c r="V17" t="str">
-        <v>Full Stack Developer</v>
+        <v>Front End Developer</v>
       </c>
       <c r="W17" t="str">
         <v>IT Services &amp; Consulting</v>
@@ -1770,16 +1770,13 @@
       <c r="Y17" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z17" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA17" t="str">
-        <v>Minimum 5 years of experience in Java Full Stack Development with proficiency in front-end technologies | Lead design, build, and configuration of applications; collaborate with teams and ensure timely delivery</v>
+        <v>3+ years of experience in .NET technologies, strong expertise in C# and Web APIs, and knowledge of React | Design, develop, and maintain web applications; develop RESTful APIs; collaborate with teams to deliver new features</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2026-01-09T21:47:16.925Z</v>
+        <v>2026-01-11T12:39:16.899Z</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1788,7 +1785,7 @@
         <v>17/20</v>
       </c>
       <c r="D18" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-hyderabad-3-to-8-years-090126931441</v>
+        <v>https://www.naukri.com/job-listings-software-engineers-in-canada-australia-germany-abroad-pathway-immigration-consultant-australia-canada-germany-3-to-8-years-100126014573</v>
       </c>
       <c r="E18" t="str">
         <v>Yes</v>
@@ -1797,28 +1794,28 @@
         <v>Yes</v>
       </c>
       <c r="G18" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="H18" t="str">
         <v>Yes</v>
       </c>
       <c r="I18" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J18" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K18" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L18" t="str">
         <v>Skipped</v>
       </c>
       <c r="M18" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Software Engineers in Canada | Australia | Germany</v>
       </c>
       <c r="N18" t="str">
-        <v>Accenture</v>
+        <v>Abroad Pathway Immigration Consultant</v>
       </c>
       <c r="O18" t="str">
         <v>3 - 8 years</v>
@@ -1827,22 +1824,25 @@
         <v>Not Disclosed</v>
       </c>
       <c r="Q18" t="str">
-        <v>Hyderabad</v>
+        <v>Australia</v>
       </c>
       <c r="R18" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S18" t="str">
-        <v>Less than 10</v>
+        <v>32</v>
+      </c>
+      <c r="T18" t="str">
+        <v>100+</v>
       </c>
       <c r="U18" t="str">
-        <v>software engineer, front end, css, full stack development, version control, front end technologies, javascript, code quality, nosql, sql, spring boot, database management, java, git, full stack, software solutions, html, agile, nosql databases</v>
+        <v>Technical Lead, Back End Developer, Full Stack Developer, Software Engineering, Front End Developer, Application Programming, C#, Java, C++, SDLC, Application Development, Embedded Systems Engineer, Django, .Net, Software Design, Automation Architect, Software Programming, Python</v>
       </c>
       <c r="V18" t="str">
-        <v>Full Stack Developer</v>
+        <v>Software Development - Other</v>
       </c>
       <c r="W18" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Legal</v>
       </c>
       <c r="X18" t="str">
         <v>Full Time, Permanent</v>
@@ -1854,12 +1854,12 @@
         <v>3.7</v>
       </c>
       <c r="AA18" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development; proficiency in front-end technologies and database management | Develop custom software solutions, collaborate with teams, conduct code reviews</v>
+        <v>Experienced software engineer proficient in Java, Python, and C++ | Design, develop, and deploy high-quality software solutions while collaborating with cross-functional teams | Competitive pay and growth-focused benefits</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2026-01-09T21:47:20.178Z</v>
+        <v>2026-01-11T12:39:20.129Z</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1868,13 +1868,13 @@
         <v>18/20</v>
       </c>
       <c r="D19" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-gurugram-3-to-8-years-090126931749</v>
+        <v>https://www.naukri.com/job-listings-application-developer-tv-distribution-mumbai-2-to-5-years-100126010034</v>
       </c>
       <c r="E19" t="str">
         <v>Yes</v>
       </c>
       <c r="F19" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="G19" t="str">
         <v>Yes</v>
@@ -1883,46 +1883,49 @@
         <v>Yes</v>
       </c>
       <c r="I19" t="str">
-        <v>4/undefined</v>
+        <v>3/undefined</v>
       </c>
       <c r="J19" t="str">
-        <v>Good Match</v>
+        <v>Poor Match</v>
       </c>
       <c r="K19" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L19" t="str">
         <v>Skipped</v>
       </c>
       <c r="M19" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Application Developer</v>
       </c>
       <c r="N19" t="str">
-        <v>Accenture</v>
+        <v>Free Tv Distribution</v>
       </c>
       <c r="O19" t="str">
-        <v>3 - 8 years</v>
+        <v>2 - 5 years</v>
       </c>
       <c r="P19" t="str">
-        <v>Not Disclosed</v>
+        <v>6-8.4 Lacs P.A.</v>
       </c>
       <c r="Q19" t="str">
-        <v>Gurugram</v>
+        <v>Mumbai( Andheri East )</v>
       </c>
       <c r="R19" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S19" t="str">
-        <v>Less than 10</v>
+        <v>1</v>
+      </c>
+      <c r="T19" t="str">
+        <v>50+</v>
       </c>
       <c r="U19" t="str">
-        <v>software engineer, front end, application developer, restful, web services, version control, business processes, react, angular, database management, java, git, postgresql, full stack, software solutions, debugging, construction, mysql, agile</v>
+        <v>Application Development, Ios Development, kotlin, Android Tv, Ott, Java, Firebase, Samsung Ims</v>
       </c>
       <c r="V19" t="str">
         <v>Full Stack Developer</v>
       </c>
       <c r="W19" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Telecom / ISP</v>
       </c>
       <c r="X19" t="str">
         <v>Full Time, Permanent</v>
@@ -1930,16 +1933,13 @@
       <c r="Y19" t="str">
         <v>Software Development</v>
       </c>
-      <c r="Z19" t="str">
-        <v>3.7</v>
-      </c>
       <c r="AA19" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in RESTful web services and API integration | Develop custom software solutions, collaborate with teams, and ensure application performance</v>
+        <v>Experience in Kotlin/Java for Android TV and specialization in React Native | Maintain high-performance video applications across major Smart TV platforms like Samsung, LG, and Amazon</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2026-01-09T21:47:23.460Z</v>
+        <v>2026-01-11T12:39:23.472Z</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1948,7 +1948,7 @@
         <v>19/20</v>
       </c>
       <c r="D20" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-bengaluru-3-to-8-years-090126930586</v>
+        <v>https://www.naukri.com/job-listings-senior-engineer-automation-great-west-global-business-services-bengaluru-3-to-8-years-110126005070</v>
       </c>
       <c r="E20" t="str">
         <v>Yes</v>
@@ -1969,16 +1969,16 @@
         <v>Good Match</v>
       </c>
       <c r="K20" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L20" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M20" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Senior Engineer Automation</v>
       </c>
       <c r="N20" t="str">
-        <v>Accenture</v>
+        <v>Empower</v>
       </c>
       <c r="O20" t="str">
         <v>3 - 8 years</v>
@@ -1990,36 +1990,36 @@
         <v>Bengaluru</v>
       </c>
       <c r="R20" t="str">
-        <v>1 day ago</v>
+        <v>Today</v>
       </c>
       <c r="S20" t="str">
-        <v>Less than 10</v>
+        <v>100+</v>
       </c>
       <c r="U20" t="str">
-        <v>software engineer, css, restful, react, sql, microservices, java, git, webpack, kanban, web development, azure, front end, oracle, software development, npm, javascript, sql server, angular, spring boot, restful apis, full stack, babel, scrum, agile</v>
+        <v>automation framework, rest, kubernetes, automation testing, cucumber, rbac, distribution system, software quality, selenium webdriver, microsoft, microservices, salesforce, environment, java, automation, selenium, json, microsoft graph, webdriver, typescript, api, gherkin, crm</v>
       </c>
       <c r="V20" t="str">
-        <v>Full Stack Developer</v>
+        <v>Automation Test Engineer</v>
       </c>
       <c r="W20" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Financial Services</v>
       </c>
       <c r="X20" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y20" t="str">
-        <v>Software Development</v>
+        <v>Quality Assurance and Testing</v>
       </c>
       <c r="Z20" t="str">
-        <v>3.7</v>
+        <v>4.0</v>
       </c>
       <c r="AA20" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with strong proficiency in Java and React.js | Design, develop, and maintain Java-based applications and microservices; collaborate with teams to deliver high-quality software</v>
+        <v>5-8+ years in software quality and test automation; strong proficiency in Java and TypeScript; experience with Gherkin/Cucumber and Selenium WebDriver | Drive quality execution across microservices; build and extend automation frameworks; perform manual and exploratory testing</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2026-01-09T21:47:26.839Z</v>
+        <v>2026-01-11T12:39:52.036Z</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2028,7 +2028,7 @@
         <v>20/20</v>
       </c>
       <c r="D21" t="str">
-        <v>https://www.naukri.com/job-listings-custom-software-engineer-accenture-solutions-pvt-ltd-pune-3-to-8-years-090126931252</v>
+        <v>https://www.naukri.com/job-listings-ground-station-engineer-adani-group-hyderabad-3-to-7-years-100126017209</v>
       </c>
       <c r="E21" t="str">
         <v>Yes</v>
@@ -2049,52 +2049,52 @@
         <v>Good Match</v>
       </c>
       <c r="K21" t="str">
-        <v>External Apply</v>
+        <v>Direct Apply</v>
       </c>
       <c r="L21" t="str">
-        <v>Skipped</v>
+        <v>Applied</v>
       </c>
       <c r="M21" t="str">
-        <v>Custom Software Engineer</v>
+        <v>Ground Station Engineer</v>
       </c>
       <c r="N21" t="str">
-        <v>Accenture</v>
+        <v>Adani Group</v>
       </c>
       <c r="O21" t="str">
-        <v>3 - 8 years</v>
+        <v>3 - 7 years</v>
       </c>
       <c r="P21" t="str">
         <v>Not Disclosed</v>
       </c>
       <c r="Q21" t="str">
-        <v>Pune</v>
+        <v>Hyderabad</v>
       </c>
       <c r="R21" t="str">
         <v>1 day ago</v>
       </c>
       <c r="S21" t="str">
-        <v>Less than 10</v>
+        <v>33</v>
       </c>
       <c r="U21" t="str">
-        <v>software engineer, rest, css, rest api design, react, backend development, javascript, nosql, sql, docker, java, testing frameworks, api design, gcp, devops, full stack, software solutions, gitlab, typescript, agile, aws, azure, agile methodology</v>
+        <v>kubernetes, python, project management, electronics, sonarqube, plc, monitoring, scada, commissioning, sql server, ospf, docker, electricals, kafka, installation, scrum, telemetry, mysql, agile, aws, jira, agile methodology, architecture</v>
       </c>
       <c r="V21" t="str">
-        <v>Search Engineer</v>
+        <v>Transportation Engineer</v>
       </c>
       <c r="W21" t="str">
-        <v>IT Services &amp; Consulting</v>
+        <v>Defence &amp; Aerospace</v>
       </c>
       <c r="X21" t="str">
         <v>Full Time, Permanent</v>
       </c>
       <c r="Y21" t="str">
-        <v>Software Development</v>
+        <v>Construction Engineering</v>
       </c>
       <c r="Z21" t="str">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="AA21" t="str">
-        <v>Minimum 3 years of experience in Java Full Stack Development with proficiency in frontend and backend technologies | Develop custom software solutions, collaborate with teams, mentor junior members, and facilitate knowledge sharing</v>
+        <v>B Tech in electronics/electrical/mechanical with 2+ years of GCS development experience | Integrate GCS/MCS software, ensure technician training, and maintain GCS/MCS schedules</v>
       </c>
     </row>
   </sheetData>

</xml_diff>